<commit_message>
Excel Tabelle um Spielprotokoll ergänzen
</commit_message>
<xml_diff>
--- a/Spielfeld/IncidentResponse-TableTop-AllesInExcel.xlsx
+++ b/Spielfeld/IncidentResponse-TableTop-AllesInExcel.xlsx
@@ -8,19 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steffen.arnold\Desktop\Dokumente\Konzepte Ideen &amp; Wissen\Notfallmanagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC144FE8-30DB-4E97-806F-B037533ABDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC42D2F-D9DB-45F4-B0CD-0FEEA469ECD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{1C5285D5-E20F-439F-859B-4E198725EEBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Spielanleitung" sheetId="2" r:id="rId1"/>
     <sheet name="Spielfeld" sheetId="1" r:id="rId2"/>
-    <sheet name="Aktionen" sheetId="4" r:id="rId3"/>
-    <sheet name="Infektionspfade" sheetId="5" r:id="rId4"/>
-    <sheet name="Szenarien" sheetId="3" r:id="rId5"/>
+    <sheet name="Spielprotokoll Angreifer" sheetId="6" r:id="rId3"/>
+    <sheet name="Spielprotokoll Verteidiger" sheetId="7" r:id="rId4"/>
+    <sheet name="Aktionen" sheetId="4" r:id="rId5"/>
+    <sheet name="Infektionspfade" sheetId="5" r:id="rId6"/>
+    <sheet name="Szenarien" sheetId="3" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Infektionspfade!$C$5:$H$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Infektionspfade!$C$5:$H$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Infektionspfade!$C$5:$H$46</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="302">
   <si>
     <t>📌 Spielanleitung für die Incident-Response-Tabletop-Übung</t>
   </si>
@@ -379,9 +382,6 @@
     <t>Verteidiger</t>
   </si>
   <si>
-    <t>Scannen / Alarme prüfen</t>
-  </si>
-  <si>
     <t>Verteidiger / Angreifer</t>
   </si>
   <si>
@@ -406,46 +406,28 @@
     <t>Scannt ein System auf Infektion (Ergebnis in der nächsten Runde).</t>
   </si>
   <si>
-    <t>Isolieren</t>
-  </si>
-  <si>
     <t>2 AE</t>
   </si>
   <si>
-    <t>Passwort zurücksetzen</t>
-  </si>
-  <si>
     <t>Account kann nicht mehr genutzt werden. </t>
   </si>
   <si>
     <t>Das Passwort eines Accounts wird zurückgesetzt. Es kann nicht mehr für Angriffe genutzt werden. </t>
-  </si>
-  <si>
-    <t>Forensik</t>
   </si>
   <si>
     <t xml:space="preserve">Ein Infektionspfad wird offengelegt.
 Muss von einer bereits identifizierten Infektion ausgehen. </t>
   </si>
   <si>
-    <t>Patchen</t>
-  </si>
-  <si>
     <t>Infektions-Kosten werden verdreifacht.</t>
   </si>
   <si>
     <t>Behebt eine Schwachstelle.  </t>
   </si>
   <si>
-    <t>Infizieren / Remote Code Execution / Lateral Movement</t>
-  </si>
-  <si>
     <t>Die Verteidiger müssen nun auf ihrem Verteidigerbrett nach diesem System/Benutzer suchen.</t>
   </si>
   <si>
-    <t>Verschlüsselung</t>
-  </si>
-  <si>
     <t>Erfolgreich infizierte Systeme werden verschlüsselt. Sie stehen nicht mehr für die Verteidigung bereit. </t>
   </si>
   <si>
@@ -459,9 +441,6 @@
   </si>
   <si>
     <t>Aktionen für die das System gebraucht wird schlagen fehl. </t>
-  </si>
-  <si>
-    <t>Obfuscation</t>
   </si>
   <si>
     <t>Der Angreifer manipuliert Logs oder andere Systemdaten, um die Verteidiger in die Irre zu führen.</t>
@@ -1031,6 +1010,96 @@
   </si>
   <si>
     <t>öffentlich / extern</t>
+  </si>
+  <si>
+    <t>Runde</t>
+  </si>
+  <si>
+    <t>System / Zone</t>
+  </si>
+  <si>
+    <t>Status vorher</t>
+  </si>
+  <si>
+    <t>Aktion Verteidiger</t>
+  </si>
+  <si>
+    <t>Aktion Angreifer</t>
+  </si>
+  <si>
+    <t>Status nachher</t>
+  </si>
+  <si>
+    <t>Webserver (DMZ)</t>
+  </si>
+  <si>
+    <t>AD-Server (Zone 1)</t>
+  </si>
+  <si>
+    <t>🔥 Escalation</t>
+  </si>
+  <si>
+    <t>🛑 Isolieren</t>
+  </si>
+  <si>
+    <t>Gesund</t>
+  </si>
+  <si>
+    <t>Infiziert</t>
+  </si>
+  <si>
+    <t>Kritisch</t>
+  </si>
+  <si>
+    <t>Infiziert (1x)</t>
+  </si>
+  <si>
+    <t>Infiziert (bleibt)</t>
+  </si>
+  <si>
+    <t>Isoliert</t>
+  </si>
+  <si>
+    <t>Kritisch (2x)</t>
+  </si>
+  <si>
+    <t>Zone übernommen</t>
+  </si>
+  <si>
+    <t>Infektionspfad</t>
+  </si>
+  <si>
+    <t>Webserver (Zone 3)</t>
+  </si>
+  <si>
+    <t>Server (Zone 2)</t>
+  </si>
+  <si>
+    <t>Infrastruktur Übernommen</t>
+  </si>
+  <si>
+    <t>📷 Forensik</t>
+  </si>
+  <si>
+    <t>🔒Passwort zurücksetzen</t>
+  </si>
+  <si>
+    <t>🎭 Obfuscation</t>
+  </si>
+  <si>
+    <t>☠ Verschlüsselung</t>
+  </si>
+  <si>
+    <t>🏹 Infizieren / Remote Code Execution / Lateral Movement</t>
+  </si>
+  <si>
+    <t>🔧 Patchen</t>
+  </si>
+  <si>
+    <t>🔍 Scannen / Alarme prüfen</t>
+  </si>
+  <si>
+    <t>Tabellarisches Protokoll für den Spiel-Ablauf 📝</t>
   </si>
 </sst>
 </file>
@@ -1253,7 +1322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1349,13 +1418,13 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1365,7 +1434,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1396,17 +1465,14 @@
     <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1425,11 +1491,26 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2842,8 +2923,35 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C286B4D5-975E-4632-829A-78172495BDFC}" name="Tabelle1" displayName="Tabelle1" ref="B4:H9" totalsRowShown="0">
+  <autoFilter ref="B4:H9" xr:uid="{C286B4D5-975E-4632-829A-78172495BDFC}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{206FF103-9523-4B9B-A0F6-EB251654F2DF}" name="Runde"/>
+    <tableColumn id="2" xr3:uid="{40FA183E-9AC3-4C74-8CBF-32DBEF652AEA}" name="System / Zone"/>
+    <tableColumn id="3" xr3:uid="{261F29AA-9550-4578-9ADC-8BBD23E3C892}" name="Status vorher"/>
+    <tableColumn id="4" xr3:uid="{12AFAC19-54B5-4F81-8CC8-3008A5413882}" name="Aktion Angreifer"/>
+    <tableColumn id="5" xr3:uid="{0E21D8D2-FA33-4623-B274-D6EDE8810B50}" name="Infektionspfad"/>
+    <tableColumn id="6" xr3:uid="{E2E1FE3B-F9FB-4A87-BD5D-F276C4DBD456}" name="Kosten"/>
+    <tableColumn id="7" xr3:uid="{373315A0-312E-4AC2-832E-F536B3C8A75B}" name="Status nachher"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{21544B41-C4BB-4153-A7A2-DB4FCE62E124}" name="Tabelle2" displayName="Tabelle2" ref="B4:G8" totalsRowShown="0">
+  <autoFilter ref="B4:G8" xr:uid="{21544B41-C4BB-4153-A7A2-DB4FCE62E124}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{193D1D85-CE9F-426A-90E9-BAE334504594}" name="Runde"/>
+    <tableColumn id="2" xr3:uid="{91030B68-A9ED-4229-8CD0-32D2AC6A8597}" name="System / Zone"/>
+    <tableColumn id="3" xr3:uid="{171F4061-1CFF-45AB-A6B3-9E1594E72F8D}" name="Status vorher"/>
+    <tableColumn id="4" xr3:uid="{CF122285-1C80-4018-9E90-2F83927FF51B}" name="Aktion Verteidiger"/>
+    <tableColumn id="5" xr3:uid="{582FD841-13E5-4626-960E-7004E8256F8F}" name="Kosten" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{FA2B43BF-0149-4F0F-9E5A-D482F6F4CB78}" name="Status nachher"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3222,7 +3330,7 @@
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.3">
@@ -3237,7 +3345,7 @@
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="22.8" x14ac:dyDescent="0.3">
@@ -3255,7 +3363,7 @@
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.3">
@@ -3265,7 +3373,7 @@
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.3">
@@ -3475,59 +3583,59 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B2" s="66" t="s">
-        <v>279</v>
-      </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="69" t="s">
-        <v>257</v>
-      </c>
-      <c r="E2" s="64"/>
-      <c r="F2" s="67" t="s">
-        <v>200</v>
-      </c>
-      <c r="G2" s="64"/>
-      <c r="H2" s="68" t="s">
-        <v>199</v>
-      </c>
-      <c r="I2" s="64"/>
-      <c r="J2" s="70" t="s">
-        <v>198</v>
+      <c r="B2" s="65" t="s">
+        <v>271</v>
+      </c>
+      <c r="C2" s="63"/>
+      <c r="D2" s="68" t="s">
+        <v>249</v>
+      </c>
+      <c r="E2" s="63"/>
+      <c r="F2" s="66" t="s">
+        <v>192</v>
+      </c>
+      <c r="G2" s="63"/>
+      <c r="H2" s="67" t="s">
+        <v>191</v>
+      </c>
+      <c r="I2" s="63"/>
+      <c r="J2" s="69" t="s">
+        <v>190</v>
       </c>
       <c r="N2" s="44" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="D3" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="F3" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="H3" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="J3" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="N3" s="45" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="O3" s="45" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="P3" s="45" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="Q3" s="45" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="R3" s="45" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -3535,164 +3643,164 @@
         <v>0</v>
       </c>
       <c r="O4" s="46" t="s">
+        <v>190</v>
+      </c>
+      <c r="P4" s="46" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q4" s="46" t="s">
         <v>198</v>
       </c>
-      <c r="P4" s="46" t="s">
+      <c r="R4" s="46" t="s">
         <v>202</v>
       </c>
-      <c r="Q4" s="46" t="s">
-        <v>206</v>
-      </c>
-      <c r="R4" s="46" t="s">
-        <v>210</v>
-      </c>
     </row>
     <row r="5" spans="1:18" ht="53.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="64" t="s">
-        <v>266</v>
+      <c r="A5" s="63" t="s">
+        <v>258</v>
       </c>
       <c r="D5" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="F5" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="H5" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="N5" s="51">
         <v>1</v>
       </c>
       <c r="O5" s="47" t="s">
+        <v>191</v>
+      </c>
+      <c r="P5" s="47" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q5" s="47" t="s">
         <v>199</v>
       </c>
-      <c r="P5" s="47" t="s">
+      <c r="R5" s="47" t="s">
         <v>203</v>
       </c>
-      <c r="Q5" s="47" t="s">
-        <v>207</v>
-      </c>
-      <c r="R5" s="47" t="s">
-        <v>211</v>
-      </c>
     </row>
     <row r="6" spans="1:18" ht="27" x14ac:dyDescent="0.3">
-      <c r="A6" s="64"/>
+      <c r="A6" s="63"/>
       <c r="N6" s="52">
         <v>2</v>
       </c>
       <c r="O6" s="48" t="s">
+        <v>192</v>
+      </c>
+      <c r="P6" s="48" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q6" s="48" t="s">
         <v>200</v>
       </c>
-      <c r="P6" s="48" t="s">
+      <c r="R6" s="48" t="s">
         <v>204</v>
       </c>
-      <c r="Q6" s="48" t="s">
-        <v>208</v>
-      </c>
-      <c r="R6" s="48" t="s">
-        <v>212</v>
-      </c>
     </row>
     <row r="7" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="65" t="s">
-        <v>269</v>
+      <c r="A7" s="64" t="s">
+        <v>261</v>
       </c>
       <c r="N7" s="53">
         <v>3</v>
       </c>
       <c r="O7" s="49" t="s">
+        <v>193</v>
+      </c>
+      <c r="P7" s="49" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q7" s="49" t="s">
         <v>201</v>
       </c>
-      <c r="P7" s="49" t="s">
+      <c r="R7" s="49" t="s">
         <v>205</v>
       </c>
-      <c r="Q7" s="49" t="s">
-        <v>209</v>
-      </c>
-      <c r="R7" s="49" t="s">
-        <v>213</v>
-      </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="64"/>
-      <c r="N8" s="62">
+      <c r="A8" s="63"/>
+      <c r="N8" s="61">
         <v>4</v>
       </c>
-      <c r="O8" s="63" t="s">
+      <c r="O8" s="62" t="s">
+        <v>246</v>
+      </c>
+      <c r="P8" s="62" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q8" s="62" t="s">
+        <v>247</v>
+      </c>
+      <c r="R8" s="62" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="63"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" s="63"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="63" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" s="63"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="63"/>
+      <c r="F13" t="s">
+        <v>266</v>
+      </c>
+      <c r="H13" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" s="63"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="63"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" s="63" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="63"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="63"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="63"/>
+      <c r="D19" t="s">
+        <v>246</v>
+      </c>
+      <c r="F19" t="s">
+        <v>253</v>
+      </c>
+      <c r="H19" t="s">
         <v>254</v>
       </c>
-      <c r="P8" s="63" t="s">
-        <v>256</v>
-      </c>
-      <c r="Q8" s="63" t="s">
+      <c r="J19" t="s">
         <v>255</v>
       </c>
-      <c r="R8" s="63" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="64"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="64"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="64" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="64"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="64"/>
-      <c r="F13" t="s">
-        <v>274</v>
-      </c>
-      <c r="H13" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="64"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="64"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="64" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="64"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="64"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="64"/>
-      <c r="D19" t="s">
-        <v>254</v>
-      </c>
-      <c r="F19" t="s">
-        <v>261</v>
-      </c>
-      <c r="H19" t="s">
-        <v>262</v>
-      </c>
-      <c r="J19" t="s">
-        <v>263</v>
-      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="64"/>
+      <c r="A20" s="63"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="64" t="s">
-        <v>253</v>
+      <c r="A21" s="63" t="s">
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -3703,50 +3811,343 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B9BCE30-3ECA-4C41-8566-5E2EE642E8AA}">
+  <dimension ref="B2:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="21.5546875" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="39" customWidth="1"/>
+    <col min="6" max="6" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="8" max="8" width="23.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="B2" s="38" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="B3" s="38"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>272</v>
+      </c>
+      <c r="C4" t="s">
+        <v>273</v>
+      </c>
+      <c r="D4" t="s">
+        <v>274</v>
+      </c>
+      <c r="E4" t="s">
+        <v>276</v>
+      </c>
+      <c r="F4" t="s">
+        <v>290</v>
+      </c>
+      <c r="G4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>291</v>
+      </c>
+      <c r="D5" t="s">
+        <v>282</v>
+      </c>
+      <c r="E5" s="73" t="s">
+        <v>298</v>
+      </c>
+      <c r="F5" t="s">
+        <v>107</v>
+      </c>
+      <c r="G5" s="74">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>292</v>
+      </c>
+      <c r="D6" t="s">
+        <v>282</v>
+      </c>
+      <c r="E6" s="73" t="s">
+        <v>298</v>
+      </c>
+      <c r="F6" t="s">
+        <v>161</v>
+      </c>
+      <c r="G6" s="74">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>279</v>
+      </c>
+      <c r="D7" t="s">
+        <v>284</v>
+      </c>
+      <c r="E7" s="73" t="s">
+        <v>298</v>
+      </c>
+      <c r="F7" t="s">
+        <v>161</v>
+      </c>
+      <c r="G7" s="74">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8" s="71" t="s">
+        <v>279</v>
+      </c>
+      <c r="D8" s="71" t="s">
+        <v>282</v>
+      </c>
+      <c r="E8" s="73" t="s">
+        <v>280</v>
+      </c>
+      <c r="F8" t="s">
+        <v>206</v>
+      </c>
+      <c r="G8" s="74">
+        <v>2</v>
+      </c>
+      <c r="H8" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="71"/>
+      <c r="G9" s="71"/>
+      <c r="H9" s="71"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAC2E9B2-0D72-456D-A45F-C7AB909482C9}">
+  <dimension ref="B2:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5546875" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" customWidth="1"/>
+    <col min="7" max="7" width="16.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="B2" s="38" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>272</v>
+      </c>
+      <c r="C4" t="s">
+        <v>273</v>
+      </c>
+      <c r="D4" t="s">
+        <v>274</v>
+      </c>
+      <c r="E4" t="s">
+        <v>275</v>
+      </c>
+      <c r="F4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>278</v>
+      </c>
+      <c r="D5" t="s">
+        <v>282</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>300</v>
+      </c>
+      <c r="F5" s="74">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>278</v>
+      </c>
+      <c r="D6" t="s">
+        <v>283</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>299</v>
+      </c>
+      <c r="F6" s="74">
+        <v>2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>278</v>
+      </c>
+      <c r="D7" t="s">
+        <v>283</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>281</v>
+      </c>
+      <c r="F7" s="74">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>279</v>
+      </c>
+      <c r="D8" t="s">
+        <v>282</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>294</v>
+      </c>
+      <c r="F8" s="74">
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>289</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3594A00-04B0-43C4-9C3C-80CBB3A4F164}">
-  <dimension ref="B3:G36"/>
+  <dimension ref="B1:G36"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="19.77734375" customWidth="1"/>
     <col min="3" max="3" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.88671875" customWidth="1"/>
+    <col min="4" max="4" width="23.109375" style="72" customWidth="1"/>
     <col min="5" max="5" width="20.5546875" customWidth="1"/>
     <col min="6" max="6" width="89.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="60.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D1"/>
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="D2"/>
+    </row>
     <row r="3" spans="2:7" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B3" s="38" t="s">
-        <v>95</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="D3"/>
     </row>
     <row r="4" spans="2:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B4" s="31"/>
+      <c r="D4"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="32" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C5" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="E5" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="F5" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="F5" s="32" t="s">
+      <c r="G5" s="32" t="s">
         <v>67</v>
-      </c>
-      <c r="G5" s="32" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
@@ -3755,16 +4156,16 @@
         <v>62</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>63</v>
+        <v>300</v>
       </c>
       <c r="E6" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="F6" s="35" t="s">
+      <c r="G6" s="35" t="s">
         <v>70</v>
-      </c>
-      <c r="G6" s="35" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
@@ -3773,16 +4174,16 @@
         <v>62</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>72</v>
+        <v>281</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F7" s="36" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="G7" s="36" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
@@ -3791,16 +4192,16 @@
         <v>62</v>
       </c>
       <c r="D8" s="35" t="s">
-        <v>74</v>
+        <v>295</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F8" s="35" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G8" s="35" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
@@ -3809,16 +4210,16 @@
         <v>62</v>
       </c>
       <c r="D9" s="35" t="s">
-        <v>77</v>
+        <v>294</v>
       </c>
       <c r="E9" s="33" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F9" s="35" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="G9" s="35" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
@@ -3827,106 +4228,106 @@
         <v>62</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>79</v>
+        <v>299</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F10" s="35" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G10" s="35" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="34"/>
       <c r="C11" s="34" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>82</v>
+        <v>298</v>
       </c>
       <c r="E11" s="34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F11" s="37" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="G11" s="37" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="34"/>
       <c r="C12" s="34" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>84</v>
+        <v>297</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F12" s="37" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="G12" s="37" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="34"/>
       <c r="C13" s="34" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E13" s="34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F13" s="37" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G13" s="37" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="34"/>
       <c r="C14" s="34" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>90</v>
+        <v>296</v>
       </c>
       <c r="E14" s="34" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F14" s="37" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="G14" s="37" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="34"/>
       <c r="C15" s="34" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D15" s="37" t="s">
-        <v>93</v>
+        <v>280</v>
       </c>
       <c r="E15" s="34" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F15" s="37" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="G15" s="37" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" ht="35.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3951,12 +4352,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{386C6478-7A38-416C-920B-C0FC0A8E8C29}">
   <dimension ref="B3:H46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="53.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3971,785 +4372,790 @@
   <sheetData>
     <row r="3" spans="2:8" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B3" s="38" t="s">
-        <v>244</v>
-      </c>
-      <c r="D3" s="57"/>
-      <c r="E3" s="58"/>
+        <v>236</v>
+      </c>
+      <c r="D3" s="56"/>
+      <c r="E3" s="57"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C5" s="40" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D5" s="40" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="E5" s="40" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="F5" s="40" t="s">
-        <v>105</v>
-      </c>
-      <c r="G5" s="59" t="s">
-        <v>245</v>
-      </c>
-      <c r="H5" s="59" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" ht="42" x14ac:dyDescent="0.3">
-      <c r="C6" s="55" t="s">
-        <v>151</v>
+        <v>97</v>
+      </c>
+      <c r="G5" s="58" t="s">
+        <v>237</v>
+      </c>
+      <c r="H5" s="58" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C6" s="42" t="s">
+        <v>122</v>
       </c>
       <c r="D6" s="39" t="s">
-        <v>221</v>
+        <v>132</v>
       </c>
       <c r="E6" s="43" t="s">
-        <v>222</v>
+        <v>133</v>
       </c>
       <c r="F6" s="39" t="s">
-        <v>223</v>
+        <v>134</v>
       </c>
       <c r="G6" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="H6" s="60" t="s">
-        <v>251</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="H6" s="39"/>
     </row>
     <row r="7" spans="2:8" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="C7" s="54" t="s">
-        <v>106</v>
+      <c r="C7" s="42" t="s">
+        <v>122</v>
       </c>
       <c r="D7" s="39" t="s">
-        <v>115</v>
-      </c>
-      <c r="E7" s="54" t="s">
-        <v>116</v>
+        <v>166</v>
+      </c>
+      <c r="E7" s="43" t="s">
+        <v>216</v>
       </c>
       <c r="F7" s="39" t="s">
-        <v>117</v>
+        <v>217</v>
       </c>
       <c r="G7" s="39" t="s">
-        <v>246</v>
+        <v>85</v>
       </c>
       <c r="H7" s="39"/>
     </row>
     <row r="8" spans="2:8" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="C8" s="43" t="s">
-        <v>130</v>
+      <c r="C8" s="42" t="s">
+        <v>122</v>
       </c>
       <c r="D8" s="39" t="s">
-        <v>140</v>
+        <v>206</v>
       </c>
       <c r="E8" s="43" t="s">
-        <v>141</v>
+        <v>207</v>
       </c>
       <c r="F8" s="39" t="s">
-        <v>142</v>
+        <v>208</v>
       </c>
       <c r="G8" s="39" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="H8" s="39"/>
     </row>
     <row r="9" spans="2:8" ht="28.2" x14ac:dyDescent="0.3">
       <c r="C9" s="42" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="D9" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="E9" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="F9" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="G9" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="H9" s="39"/>
+    </row>
+    <row r="10" spans="2:8" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="C10" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="D10" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="E10" s="43" t="s">
+        <v>227</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>228</v>
+      </c>
+      <c r="G10" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="H10" s="59" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="C11" s="54" t="s">
+        <v>177</v>
+      </c>
+      <c r="D11" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="E11" s="55" t="s">
+        <v>111</v>
+      </c>
+      <c r="F11" s="39" t="s">
+        <v>152</v>
+      </c>
+      <c r="G11" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="H11" s="39"/>
+    </row>
+    <row r="12" spans="2:8" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="C12" s="54" t="s">
+        <v>178</v>
+      </c>
+      <c r="D12" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="E12" s="55" t="s">
         <v>143</v>
       </c>
-      <c r="E9" s="42" t="s">
-        <v>144</v>
-      </c>
-      <c r="F9" s="39" t="s">
-        <v>145</v>
-      </c>
-      <c r="G9" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="H9" s="39"/>
-    </row>
-    <row r="10" spans="2:8" ht="55.8" x14ac:dyDescent="0.3">
-      <c r="C10" s="54" t="s">
-        <v>185</v>
-      </c>
-      <c r="D10" s="39" t="s">
-        <v>159</v>
-      </c>
-      <c r="E10" s="55" t="s">
-        <v>119</v>
-      </c>
-      <c r="F10" s="39" t="s">
-        <v>160</v>
-      </c>
-      <c r="G10" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="H10" s="39"/>
-    </row>
-    <row r="11" spans="2:8" ht="42" x14ac:dyDescent="0.3">
-      <c r="C11" s="54" t="s">
-        <v>106</v>
-      </c>
-      <c r="D11" s="39" t="s">
-        <v>118</v>
-      </c>
-      <c r="E11" s="55" t="s">
-        <v>119</v>
-      </c>
-      <c r="F11" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="G11" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="H11" s="39"/>
-    </row>
-    <row r="12" spans="2:8" ht="42" x14ac:dyDescent="0.3">
-      <c r="C12" s="55" t="s">
-        <v>107</v>
-      </c>
-      <c r="D12" s="39" t="s">
-        <v>121</v>
-      </c>
-      <c r="E12" s="55" t="s">
-        <v>119</v>
-      </c>
       <c r="F12" s="39" t="s">
-        <v>122</v>
+        <v>154</v>
       </c>
       <c r="G12" s="39" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="H12" s="39"/>
     </row>
     <row r="13" spans="2:8" ht="42" x14ac:dyDescent="0.3">
       <c r="C13" s="54" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="D13" s="39" t="s">
+        <v>148</v>
+      </c>
+      <c r="E13" s="55" t="s">
+        <v>99</v>
+      </c>
+      <c r="F13" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="G13" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="H13" s="39"/>
+    </row>
+    <row r="14" spans="2:8" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="C14" s="54" t="s">
+        <v>176</v>
+      </c>
+      <c r="D14" s="39" t="s">
+        <v>161</v>
+      </c>
+      <c r="E14" s="42" t="s">
+        <v>122</v>
+      </c>
+      <c r="F14" s="39" t="s">
+        <v>162</v>
+      </c>
+      <c r="G14" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="H14" s="39"/>
+    </row>
+    <row r="15" spans="2:8" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="C15" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="D15" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="E15" s="55" t="s">
+        <v>143</v>
+      </c>
+      <c r="F15" s="39" t="s">
+        <v>144</v>
+      </c>
+      <c r="G15" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="H15" s="39"/>
+    </row>
+    <row r="16" spans="2:8" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="C16" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="D16" s="39" t="s">
+        <v>145</v>
+      </c>
+      <c r="E16" s="42" t="s">
+        <v>146</v>
+      </c>
+      <c r="F16" s="39" t="s">
+        <v>147</v>
+      </c>
+      <c r="G16" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="H16" s="39"/>
+    </row>
+    <row r="17" spans="3:8" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="C17" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="D17" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="E17" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="F17" s="39" t="s">
+        <v>155</v>
+      </c>
+      <c r="G17" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="H17" s="39"/>
+    </row>
+    <row r="18" spans="3:8" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="C18" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="D18" s="39" t="s">
+        <v>172</v>
+      </c>
+      <c r="E18" s="43" t="s">
+        <v>173</v>
+      </c>
+      <c r="F18" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="G18" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="H18" s="39"/>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C19" s="54" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="E19" s="54" t="s">
+        <v>108</v>
+      </c>
+      <c r="F19" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="G19" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="H19" s="39"/>
+    </row>
+    <row r="20" spans="3:8" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="C20" s="54" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" s="39" t="s">
+        <v>110</v>
+      </c>
+      <c r="E20" s="55" t="s">
+        <v>111</v>
+      </c>
+      <c r="F20" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="G20" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="H20" s="39"/>
+    </row>
+    <row r="21" spans="3:8" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="C21" s="54" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="E21" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="F21" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="G21" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="H21" s="39"/>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C22" s="60" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="E22" s="70" t="s">
+        <v>105</v>
+      </c>
+      <c r="F22" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="G22" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="H22" s="39"/>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C23" s="54" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" s="39" t="s">
+        <v>181</v>
+      </c>
+      <c r="E23" s="42" t="s">
+        <v>182</v>
+      </c>
+      <c r="F23" s="39" t="s">
+        <v>183</v>
+      </c>
+      <c r="G23" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="H23" s="59" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C24" s="54" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" s="39" t="s">
+        <v>101</v>
+      </c>
+      <c r="E24" s="54" t="s">
+        <v>102</v>
+      </c>
+      <c r="F24" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="G24" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="H24" s="39"/>
+    </row>
+    <row r="25" spans="3:8" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="C25" s="55" t="s">
+        <v>157</v>
+      </c>
+      <c r="D25" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="E25" s="43" t="s">
+        <v>209</v>
+      </c>
+      <c r="F25" s="39" t="s">
+        <v>218</v>
+      </c>
+      <c r="G25" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="H25" s="39"/>
+    </row>
+    <row r="26" spans="3:8" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="C26" s="55" t="s">
+        <v>143</v>
+      </c>
+      <c r="D26" s="39" t="s">
+        <v>213</v>
+      </c>
+      <c r="E26" s="43" t="s">
+        <v>214</v>
+      </c>
+      <c r="F26" s="39" t="s">
+        <v>215</v>
+      </c>
+      <c r="G26" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="H26" s="59" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="27" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C27" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="D27" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="E27" s="42" t="s">
+        <v>139</v>
+      </c>
+      <c r="F27" s="39" t="s">
+        <v>140</v>
+      </c>
+      <c r="G27" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="H27" s="39"/>
+    </row>
+    <row r="28" spans="3:8" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="C28" s="42" t="s">
+        <v>125</v>
+      </c>
+      <c r="D28" s="39" t="s">
+        <v>127</v>
+      </c>
+      <c r="E28" s="42" t="s">
+        <v>128</v>
+      </c>
+      <c r="F28" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="G28" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="H28" s="39"/>
+    </row>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C29" s="42" t="s">
+        <v>125</v>
+      </c>
+      <c r="D29" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="E29" s="55" t="s">
+        <v>179</v>
+      </c>
+      <c r="F29" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="G29" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="H29" s="39"/>
+    </row>
+    <row r="30" spans="3:8" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="C30" s="42" t="s">
+        <v>125</v>
+      </c>
+      <c r="D30" s="39" t="s">
+        <v>229</v>
+      </c>
+      <c r="E30" s="43" t="s">
+        <v>209</v>
+      </c>
+      <c r="F30" s="39" t="s">
+        <v>230</v>
+      </c>
+      <c r="G30" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="H30" s="39"/>
+    </row>
+    <row r="31" spans="3:8" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="C31" s="42" t="s">
+        <v>125</v>
+      </c>
+      <c r="D31" s="39" t="s">
+        <v>148</v>
+      </c>
+      <c r="E31" s="43" t="s">
+        <v>209</v>
+      </c>
+      <c r="F31" s="39" t="s">
+        <v>210</v>
+      </c>
+      <c r="G31" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="H31" s="39"/>
+    </row>
+    <row r="32" spans="3:8" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="C32" s="42" t="s">
+        <v>239</v>
+      </c>
+      <c r="D32" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="E32" s="43" t="s">
+        <v>211</v>
+      </c>
+      <c r="F32" s="39" t="s">
+        <v>212</v>
+      </c>
+      <c r="G32" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="H32" s="39"/>
+    </row>
+    <row r="33" spans="3:8" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="C33" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="D33" s="39" t="s">
         <v>156</v>
       </c>
-      <c r="E13" s="55" t="s">
-        <v>107</v>
-      </c>
-      <c r="F13" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="G13" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="H13" s="39"/>
-    </row>
-    <row r="14" spans="2:8" ht="42" x14ac:dyDescent="0.3">
-      <c r="C14" s="54" t="s">
-        <v>106</v>
-      </c>
-      <c r="D14" s="39" t="s">
-        <v>188</v>
-      </c>
-      <c r="E14" s="42" t="s">
-        <v>107</v>
-      </c>
-      <c r="F14" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="G14" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="H14" s="39"/>
-    </row>
-    <row r="15" spans="2:8" ht="42" x14ac:dyDescent="0.3">
-      <c r="C15" s="54" t="s">
-        <v>106</v>
-      </c>
-      <c r="D15" s="39" t="s">
-        <v>112</v>
-      </c>
-      <c r="E15" s="55" t="s">
+      <c r="E33" s="55" t="s">
+        <v>179</v>
+      </c>
+      <c r="F33" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="G33" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="H33" s="39"/>
+    </row>
+    <row r="34" spans="3:8" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="C34" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="D34" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="E34" s="42" t="s">
+        <v>122</v>
+      </c>
+      <c r="F34" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="G34" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="H34" s="39"/>
+    </row>
+    <row r="35" spans="3:8" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="C35" s="43" t="s">
+        <v>231</v>
+      </c>
+      <c r="D35" s="39" t="s">
+        <v>232</v>
+      </c>
+      <c r="E35" s="43" t="s">
+        <v>233</v>
+      </c>
+      <c r="F35" s="39" t="s">
+        <v>234</v>
+      </c>
+      <c r="G35" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="H35" s="39"/>
+    </row>
+    <row r="36" spans="3:8" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="C36" s="54" t="s">
+        <v>223</v>
+      </c>
+      <c r="D36" s="39" t="s">
+        <v>224</v>
+      </c>
+      <c r="E36" s="43" t="s">
+        <v>225</v>
+      </c>
+      <c r="F36" s="39" t="s">
+        <v>226</v>
+      </c>
+      <c r="G36" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="H36" s="59" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="37" spans="3:8" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="C37" s="55" t="s">
+        <v>99</v>
+      </c>
+      <c r="D37" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="F15" s="39" t="s">
+      <c r="E37" s="55" t="s">
+        <v>111</v>
+      </c>
+      <c r="F37" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="G15" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="H15" s="39"/>
-    </row>
-    <row r="16" spans="2:8" ht="42" x14ac:dyDescent="0.3">
-      <c r="C16" s="54" t="s">
-        <v>231</v>
-      </c>
-      <c r="D16" s="39" t="s">
-        <v>232</v>
-      </c>
-      <c r="E16" s="43" t="s">
-        <v>233</v>
-      </c>
-      <c r="F16" s="39" t="s">
-        <v>234</v>
-      </c>
-      <c r="G16" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="H16" s="60" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="17" spans="3:8" ht="42" x14ac:dyDescent="0.3">
-      <c r="C17" s="43" t="s">
-        <v>130</v>
-      </c>
-      <c r="D17" s="39" t="s">
-        <v>174</v>
-      </c>
-      <c r="E17" s="43" t="s">
-        <v>224</v>
-      </c>
-      <c r="F17" s="39" t="s">
-        <v>225</v>
-      </c>
-      <c r="G17" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="H17" s="39"/>
-    </row>
-    <row r="18" spans="3:8" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="C18" s="54" t="s">
-        <v>106</v>
-      </c>
-      <c r="D18" s="39" t="s">
-        <v>189</v>
-      </c>
-      <c r="E18" s="42" t="s">
-        <v>190</v>
-      </c>
-      <c r="F18" s="39" t="s">
-        <v>191</v>
-      </c>
-      <c r="G18" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="H18" s="60" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="19" spans="3:8" ht="42" x14ac:dyDescent="0.3">
-      <c r="C19" s="42" t="s">
-        <v>125</v>
-      </c>
-      <c r="D19" s="39" t="s">
-        <v>143</v>
-      </c>
-      <c r="E19" s="43" t="s">
-        <v>235</v>
-      </c>
-      <c r="F19" s="39" t="s">
-        <v>236</v>
-      </c>
-      <c r="G19" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="H19" s="60" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="20" spans="3:8" ht="69.599999999999994" x14ac:dyDescent="0.3">
-      <c r="C20" s="55" t="s">
-        <v>107</v>
-      </c>
-      <c r="D20" s="39" t="s">
-        <v>123</v>
-      </c>
-      <c r="E20" s="42" t="s">
-        <v>133</v>
-      </c>
-      <c r="F20" s="39" t="s">
-        <v>192</v>
-      </c>
-      <c r="G20" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="H20" s="60" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="21" spans="3:8" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="C21" s="55" t="s">
-        <v>119</v>
-      </c>
-      <c r="D21" s="39" t="s">
-        <v>132</v>
-      </c>
-      <c r="E21" s="42" t="s">
-        <v>133</v>
-      </c>
-      <c r="F21" s="39" t="s">
-        <v>134</v>
-      </c>
-      <c r="G21" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="H21" s="39"/>
-    </row>
-    <row r="22" spans="3:8" ht="42" x14ac:dyDescent="0.3">
-      <c r="C22" s="61" t="s">
-        <v>149</v>
-      </c>
-      <c r="D22" s="41" t="s">
-        <v>171</v>
-      </c>
-      <c r="E22" s="56" t="s">
-        <v>172</v>
-      </c>
-      <c r="F22" s="41" t="s">
-        <v>173</v>
-      </c>
-      <c r="G22" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="H22" s="39"/>
-    </row>
-    <row r="23" spans="3:8" ht="42" x14ac:dyDescent="0.3">
-      <c r="C23" s="54" t="s">
-        <v>186</v>
-      </c>
-      <c r="D23" s="39" t="s">
-        <v>161</v>
-      </c>
-      <c r="E23" s="55" t="s">
-        <v>151</v>
-      </c>
-      <c r="F23" s="39" t="s">
-        <v>162</v>
-      </c>
-      <c r="G23" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="H23" s="39"/>
-    </row>
-    <row r="24" spans="3:8" ht="42" x14ac:dyDescent="0.3">
-      <c r="C24" s="54" t="s">
-        <v>183</v>
-      </c>
-      <c r="D24" s="39" t="s">
-        <v>150</v>
-      </c>
-      <c r="E24" s="55" t="s">
-        <v>151</v>
-      </c>
-      <c r="F24" s="39" t="s">
-        <v>152</v>
-      </c>
-      <c r="G24" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="H24" s="39"/>
-    </row>
-    <row r="25" spans="3:8" ht="42" x14ac:dyDescent="0.3">
-      <c r="C25" s="43" t="s">
-        <v>130</v>
-      </c>
-      <c r="D25" s="39" t="s">
-        <v>214</v>
-      </c>
-      <c r="E25" s="43" t="s">
-        <v>215</v>
-      </c>
-      <c r="F25" s="39" t="s">
-        <v>216</v>
-      </c>
-      <c r="G25" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="H25" s="39"/>
-    </row>
-    <row r="26" spans="3:8" ht="42" x14ac:dyDescent="0.3">
-      <c r="C26" s="42" t="s">
-        <v>247</v>
-      </c>
-      <c r="D26" s="39" t="s">
-        <v>132</v>
-      </c>
-      <c r="E26" s="43" t="s">
-        <v>219</v>
-      </c>
-      <c r="F26" s="39" t="s">
-        <v>220</v>
-      </c>
-      <c r="G26" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="H26" s="39"/>
-    </row>
-    <row r="27" spans="3:8" ht="42" x14ac:dyDescent="0.3">
-      <c r="C27" s="43" t="s">
-        <v>239</v>
-      </c>
-      <c r="D27" s="39" t="s">
-        <v>240</v>
-      </c>
-      <c r="E27" s="43" t="s">
-        <v>241</v>
-      </c>
-      <c r="F27" s="39" t="s">
-        <v>242</v>
-      </c>
-      <c r="G27" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="H27" s="39"/>
-    </row>
-    <row r="28" spans="3:8" ht="42" x14ac:dyDescent="0.3">
-      <c r="C28" s="54" t="s">
-        <v>183</v>
-      </c>
-      <c r="D28" s="39" t="s">
-        <v>153</v>
-      </c>
-      <c r="E28" s="42" t="s">
-        <v>154</v>
-      </c>
-      <c r="F28" s="39" t="s">
-        <v>155</v>
-      </c>
-      <c r="G28" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="H28" s="39"/>
-    </row>
-    <row r="29" spans="3:8" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="C29" s="55" t="s">
-        <v>107</v>
-      </c>
-      <c r="D29" s="39" t="s">
-        <v>127</v>
-      </c>
-      <c r="E29" s="42" t="s">
-        <v>243</v>
-      </c>
-      <c r="F29" s="39" t="s">
-        <v>128</v>
-      </c>
-      <c r="G29" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="H29" s="39"/>
-    </row>
-    <row r="30" spans="3:8" ht="42" x14ac:dyDescent="0.3">
-      <c r="C30" s="42" t="s">
-        <v>133</v>
-      </c>
-      <c r="D30" s="39" t="s">
-        <v>135</v>
-      </c>
-      <c r="E30" s="42" t="s">
-        <v>136</v>
-      </c>
-      <c r="F30" s="39" t="s">
-        <v>137</v>
-      </c>
-      <c r="G30" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="H30" s="39"/>
-    </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C31" s="42" t="s">
-        <v>146</v>
-      </c>
-      <c r="D31" s="39" t="s">
-        <v>132</v>
-      </c>
-      <c r="E31" s="42" t="s">
-        <v>147</v>
-      </c>
-      <c r="F31" s="39" t="s">
-        <v>148</v>
-      </c>
-      <c r="G31" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="H31" s="39"/>
-    </row>
-    <row r="32" spans="3:8" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="C32" s="54" t="s">
-        <v>106</v>
-      </c>
-      <c r="D32" s="39" t="s">
-        <v>109</v>
-      </c>
-      <c r="E32" s="54" t="s">
-        <v>110</v>
-      </c>
-      <c r="F32" s="39" t="s">
-        <v>111</v>
-      </c>
-      <c r="G32" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="H32" s="39"/>
-    </row>
-    <row r="33" spans="3:8" ht="42" x14ac:dyDescent="0.3">
-      <c r="C33" s="54" t="s">
-        <v>183</v>
-      </c>
-      <c r="D33" s="39" t="s">
-        <v>143</v>
-      </c>
-      <c r="E33" s="42" t="s">
-        <v>125</v>
-      </c>
-      <c r="F33" s="39" t="s">
-        <v>163</v>
-      </c>
-      <c r="G33" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="H33" s="39"/>
-    </row>
-    <row r="34" spans="3:8" ht="42" x14ac:dyDescent="0.3">
-      <c r="C34" s="55" t="s">
-        <v>107</v>
-      </c>
-      <c r="D34" s="39" t="s">
-        <v>124</v>
-      </c>
-      <c r="E34" s="42" t="s">
-        <v>125</v>
-      </c>
-      <c r="F34" s="39" t="s">
-        <v>126</v>
-      </c>
-      <c r="G34" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="H34" s="39"/>
-    </row>
-    <row r="35" spans="3:8" ht="42" x14ac:dyDescent="0.3">
-      <c r="C35" s="54" t="s">
-        <v>149</v>
-      </c>
-      <c r="D35" s="39" t="s">
-        <v>176</v>
-      </c>
-      <c r="E35" s="54" t="s">
-        <v>177</v>
-      </c>
-      <c r="F35" s="39" t="s">
-        <v>178</v>
-      </c>
-      <c r="G35" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="H35" s="39"/>
-    </row>
-    <row r="36" spans="3:8" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="C36" s="42" t="s">
-        <v>133</v>
-      </c>
-      <c r="D36" s="39" t="s">
-        <v>138</v>
-      </c>
-      <c r="E36" s="55" t="s">
-        <v>187</v>
-      </c>
-      <c r="F36" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="G36" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="H36" s="39"/>
-    </row>
-    <row r="37" spans="3:8" ht="42" x14ac:dyDescent="0.3">
-      <c r="C37" s="42" t="s">
-        <v>158</v>
-      </c>
-      <c r="D37" s="39" t="s">
-        <v>164</v>
-      </c>
-      <c r="E37" s="55" t="s">
-        <v>187</v>
-      </c>
-      <c r="F37" s="39" t="s">
-        <v>166</v>
-      </c>
       <c r="G37" s="39" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="H37" s="39"/>
     </row>
     <row r="38" spans="3:8" ht="42" x14ac:dyDescent="0.3">
       <c r="C38" s="55" t="s">
+        <v>99</v>
+      </c>
+      <c r="D38" s="39" t="s">
+        <v>115</v>
+      </c>
+      <c r="E38" s="42" t="s">
+        <v>125</v>
+      </c>
+      <c r="F38" s="39" t="s">
+        <v>184</v>
+      </c>
+      <c r="G38" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="H38" s="59" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="39" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C39" s="55" t="s">
+        <v>99</v>
+      </c>
+      <c r="D39" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="E39" s="42" t="s">
+        <v>235</v>
+      </c>
+      <c r="F39" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="G39" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="H39" s="39"/>
+    </row>
+    <row r="40" spans="3:8" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="C40" s="55" t="s">
+        <v>99</v>
+      </c>
+      <c r="D40" s="39" t="s">
+        <v>116</v>
+      </c>
+      <c r="E40" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="F40" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="G40" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="H40" s="39"/>
+    </row>
+    <row r="41" spans="3:8" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="C41" s="55" t="s">
+        <v>111</v>
+      </c>
+      <c r="D41" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="E41" s="42" t="s">
+        <v>125</v>
+      </c>
+      <c r="F41" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="G41" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="H41" s="39"/>
+    </row>
+    <row r="42" spans="3:8" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="C42" s="55" t="s">
+        <v>111</v>
+      </c>
+      <c r="D42" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="E42" s="42" t="s">
+        <v>122</v>
+      </c>
+      <c r="F42" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="G42" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="H42" s="39"/>
+    </row>
+    <row r="43" spans="3:8" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="C43" s="43" t="s">
+        <v>219</v>
+      </c>
+      <c r="D43" s="39" t="s">
+        <v>220</v>
+      </c>
+      <c r="E43" s="43" t="s">
+        <v>221</v>
+      </c>
+      <c r="F43" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="G43" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="H43" s="39"/>
+    </row>
+    <row r="44" spans="3:8" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="C44" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="D44" s="39" t="s">
+        <v>163</v>
+      </c>
+      <c r="E44" s="42" t="s">
+        <v>164</v>
+      </c>
+      <c r="F44" s="39" t="s">
         <v>165</v>
       </c>
-      <c r="D38" s="39" t="s">
-        <v>127</v>
-      </c>
-      <c r="E38" s="43" t="s">
-        <v>217</v>
-      </c>
-      <c r="F38" s="39" t="s">
-        <v>226</v>
-      </c>
-      <c r="G38" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="H38" s="39"/>
-    </row>
-    <row r="39" spans="3:8" ht="55.8" x14ac:dyDescent="0.3">
-      <c r="C39" s="42" t="s">
-        <v>133</v>
-      </c>
-      <c r="D39" s="39" t="s">
-        <v>237</v>
-      </c>
-      <c r="E39" s="43" t="s">
-        <v>217</v>
-      </c>
-      <c r="F39" s="39" t="s">
+      <c r="G44" s="39" t="s">
         <v>238</v>
       </c>
-      <c r="G39" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="H39" s="39"/>
-    </row>
-    <row r="40" spans="3:8" ht="42" x14ac:dyDescent="0.3">
-      <c r="C40" s="42" t="s">
-        <v>133</v>
-      </c>
-      <c r="D40" s="39" t="s">
-        <v>156</v>
-      </c>
-      <c r="E40" s="43" t="s">
-        <v>217</v>
-      </c>
-      <c r="F40" s="39" t="s">
-        <v>218</v>
-      </c>
-      <c r="G40" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="H40" s="39"/>
-    </row>
-    <row r="41" spans="3:8" ht="42" x14ac:dyDescent="0.3">
-      <c r="C41" s="43" t="s">
-        <v>227</v>
-      </c>
-      <c r="D41" s="39" t="s">
-        <v>228</v>
-      </c>
-      <c r="E41" s="43" t="s">
-        <v>229</v>
-      </c>
-      <c r="F41" s="39" t="s">
-        <v>230</v>
-      </c>
-      <c r="G41" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="H41" s="39"/>
-    </row>
-    <row r="42" spans="3:8" ht="42" x14ac:dyDescent="0.3">
-      <c r="C42" s="42" t="s">
-        <v>179</v>
-      </c>
-      <c r="D42" s="39" t="s">
-        <v>180</v>
-      </c>
-      <c r="E42" s="43" t="s">
-        <v>181</v>
-      </c>
-      <c r="F42" s="39" t="s">
-        <v>182</v>
-      </c>
-      <c r="G42" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="H42" s="39"/>
-    </row>
-    <row r="43" spans="3:8" ht="42" x14ac:dyDescent="0.3">
-      <c r="C43" s="54" t="s">
-        <v>184</v>
-      </c>
-      <c r="D43" s="39" t="s">
+      <c r="H44" s="39"/>
+    </row>
+    <row r="45" spans="3:8" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="C45" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="D45" s="39" t="s">
+        <v>168</v>
+      </c>
+      <c r="E45" s="54" t="s">
         <v>169</v>
       </c>
-      <c r="E43" s="42" t="s">
-        <v>130</v>
-      </c>
-      <c r="F43" s="39" t="s">
+      <c r="F45" s="39" t="s">
         <v>170</v>
       </c>
-      <c r="G43" s="39" t="s">
-        <v>246</v>
-      </c>
-      <c r="H43" s="39"/>
-    </row>
-    <row r="44" spans="3:8" ht="55.8" x14ac:dyDescent="0.3">
-      <c r="C44" s="42" t="s">
-        <v>158</v>
-      </c>
-      <c r="D44" s="39" t="s">
-        <v>174</v>
-      </c>
-      <c r="E44" s="42" t="s">
-        <v>130</v>
-      </c>
-      <c r="F44" s="39" t="s">
-        <v>175</v>
-      </c>
-      <c r="G44" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="H44" s="39"/>
-    </row>
-    <row r="45" spans="3:8" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="C45" s="55" t="s">
-        <v>119</v>
-      </c>
-      <c r="D45" s="39" t="s">
-        <v>129</v>
-      </c>
-      <c r="E45" s="42" t="s">
-        <v>130</v>
-      </c>
-      <c r="F45" s="39" t="s">
-        <v>131</v>
-      </c>
       <c r="G45" s="39" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="H45" s="39"/>
     </row>
-    <row r="46" spans="3:8" ht="55.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:8" ht="28.2" x14ac:dyDescent="0.3">
       <c r="C46" s="54" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="D46" s="39" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="E46" s="42" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="F46" s="39" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="G46" s="39" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="H46" s="39"/>
     </row>
   </sheetData>
+  <autoFilter ref="C5:H46" xr:uid="{386C6478-7A38-416C-920B-C0FC0A8E8C29}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C6:H46">
+      <sortCondition ref="C5:C46"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCE6915D-FD1E-4B60-9E73-5E70C5AE7131}">
   <dimension ref="B2:F4"/>
   <sheetViews>

</xml_diff>